<commit_message>
Update DTR for Marc
</commit_message>
<xml_diff>
--- a/DTR/Marc.xlsx
+++ b/DTR/Marc.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,23 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Marc</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>15:29:19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>